<commit_message>
update Health Planner config
</commit_message>
<xml_diff>
--- a/Health-Wellness-Planner-Agent/guideline-doc.xlsx
+++ b/Health-Wellness-Planner-Agent/guideline-doc.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdulbasit.khalsai\Documents\WD\agentic-ai\beginner\repo-practice\Health-Wellness-Planner-Agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E27201E-8041-4D69-8195-F8A28282786C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68B0475-1703-4272-B9A2-35301ED53DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDF4B1E0-1388-4CE1-882E-6075E319E9EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$2:$D$99</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="165">
   <si>
     <t>Assignment Document: Health &amp; Wellness Planner Agent using OpenAI Agents SDK</t>
   </si>
@@ -1340,13 +1344,58 @@
   </si>
   <si>
     <t>End of Assignment Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi Agent </t>
+  </si>
+  <si>
+    <t>Streaming</t>
+  </si>
+  <si>
+    <t>Folder Structure</t>
+  </si>
+  <si>
+    <t>Particulars</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Handsoff</t>
+  </si>
+  <si>
+    <t>Guardrails</t>
+  </si>
+  <si>
+    <t>Past Conversation</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Through storage of chat_history in variable to be get/set user_session</t>
+  </si>
+  <si>
+    <t>interaction with natural language</t>
+  </si>
+  <si>
+    <t>Through LLM</t>
+  </si>
+  <si>
+    <t>understand goals</t>
+  </si>
+  <si>
+    <t>personalized suggestion &amp; feedback</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1424,6 +1473,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1439,9 +1496,44 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -1452,7 +1544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1494,6 +1586,19 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1833,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DC591E-24B1-4634-B810-62CC0FFF980C}">
   <dimension ref="A1:B138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A6" sqref="A1:B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2617,4 +2722,571 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303D8432-C61E-4B06-A85F-0583DA1FD4DF}">
+  <dimension ref="B2:D99"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="52.109375" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+    </row>
+    <row r="9" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B34" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B39" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B41" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B42" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B43" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B45" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B47" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B48" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B49" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B61" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B62" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B63" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B64" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B65" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B66" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B67" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B68" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B69" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B70" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B71" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B72" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B73" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B74" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B75" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B76" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B77" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B78" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B79" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B81" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B82" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B83" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B85" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B86" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B87" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B88" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B89" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B93" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>